<commit_message>
Add test cases on Home page and Profile page
</commit_message>
<xml_diff>
--- a/excel/testdata.xlsx
+++ b/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19545" windowHeight="9675" firstSheet="8" activeTab="9"/>
+    <workbookView windowWidth="19515" windowHeight="9375" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Login Test Data" sheetId="1" r:id="rId1"/>
@@ -14,16 +14,25 @@
     <sheet name="Event Test Data" sheetId="7" r:id="rId5"/>
     <sheet name="Announcement Test Data" sheetId="8" r:id="rId6"/>
     <sheet name="Search Molly Test Data" sheetId="5" r:id="rId7"/>
-    <sheet name="Personal Information Test Data" sheetId="9" r:id="rId8"/>
-    <sheet name="Contact Information Test Data" sheetId="10" r:id="rId9"/>
-    <sheet name="Educational Attainment TestData" sheetId="11" r:id="rId10"/>
+    <sheet name="ChangeProfile Picture Test Data" sheetId="20" r:id="rId8"/>
+    <sheet name="Personal Information Test Data" sheetId="9" r:id="rId9"/>
+    <sheet name="Contact Information Test Data" sheetId="10" r:id="rId10"/>
+    <sheet name="Educational Attainment TestData" sheetId="11" r:id="rId11"/>
+    <sheet name="Professional Info Test Data" sheetId="12" r:id="rId12"/>
+    <sheet name="Filter Files Test Data" sheetId="13" r:id="rId13"/>
+    <sheet name="Search Files Test Data" sheetId="14" r:id="rId14"/>
+    <sheet name="Rename File Test Data" sheetId="15" r:id="rId15"/>
+    <sheet name="Download File Test Data" sheetId="16" r:id="rId16"/>
+    <sheet name="Share File Via Link Test Data" sheetId="17" r:id="rId17"/>
+    <sheet name="Share File Via Email Test Data" sheetId="18" r:id="rId18"/>
+    <sheet name="Delete File Test Data" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="159">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -130,6 +139,30 @@
     <t>TestWithAppium</t>
   </si>
   <si>
+    <t>Profile_0002</t>
+  </si>
+  <si>
+    <t>Far far away, behind the word mountains, far from the countries Vokalia and Consonantia, there live the blind texts.</t>
+  </si>
+  <si>
+    <t>Profile_0003</t>
+  </si>
+  <si>
+    <t>Profile_0004</t>
+  </si>
+  <si>
+    <t>Profile_0005</t>
+  </si>
+  <si>
+    <t>Profile_0006</t>
+  </si>
+  <si>
+    <t>Profile_0007</t>
+  </si>
+  <si>
+    <t>A wonderful serenity has taken possession of my entire soul, like these sweet mornings of spring which I enjoy with my whole heart. I am alone, and feel the charm of existence in this spot, which was created for the bliss of souls like mine.</t>
+  </si>
+  <si>
     <t>What's this poll about?</t>
   </si>
   <si>
@@ -148,25 +181,61 @@
     <t>Home_0012</t>
   </si>
   <si>
-    <t>Test Poll</t>
-  </si>
-  <si>
-    <t>Test Choice 1</t>
-  </si>
-  <si>
-    <t>Test Choice 2</t>
+    <t>Who will people in 2030 trust more with their babies: robots or human baby-sitters?</t>
+  </si>
+  <si>
+    <t>Robots</t>
+  </si>
+  <si>
+    <t>Human baby-sitters</t>
   </si>
   <si>
     <t>Home_0013</t>
   </si>
   <si>
-    <t>Test poll more option.</t>
-  </si>
-  <si>
-    <t>Test Choice 3</t>
-  </si>
-  <si>
-    <t>Test Choice 4</t>
+    <t>What is your current role?</t>
+  </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <t>QA Tester</t>
+  </si>
+  <si>
+    <t>Web Designer</t>
+  </si>
+  <si>
+    <t>Business Development</t>
+  </si>
+  <si>
+    <t>Profile_0013</t>
+  </si>
+  <si>
+    <t>What is your age?</t>
+  </si>
+  <si>
+    <t>18 -24 years old</t>
+  </si>
+  <si>
+    <t>25 - 35 years old</t>
+  </si>
+  <si>
+    <t>Profile_0014</t>
+  </si>
+  <si>
+    <t>Have you used this app before?</t>
+  </si>
+  <si>
+    <t>Yes, I am a power user</t>
+  </si>
+  <si>
+    <t>Yes, but only a little</t>
+  </si>
+  <si>
+    <t>I’ve only seen others use it</t>
+  </si>
+  <si>
+    <t>I’ve never used or seen the application</t>
   </si>
   <si>
     <t>Category Name</t>
@@ -184,6 +253,12 @@
     <t>4986e7</t>
   </si>
   <si>
+    <t>Home_0015</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
     <t>This announcement is about</t>
   </si>
   <si>
@@ -205,6 +280,15 @@
     <t>Search Molly</t>
   </si>
   <si>
+    <t>Home_0024</t>
+  </si>
+  <si>
+    <t>Home_0025</t>
+  </si>
+  <si>
+    <t>Profile_0001</t>
+  </si>
+  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -226,7 +310,7 @@
     <t>Interests</t>
   </si>
   <si>
-    <t>Profile_0029</t>
+    <t>Profile_0030</t>
   </si>
   <si>
     <t>Mary</t>
@@ -238,6 +322,9 @@
     <t>Dela Cruz</t>
   </si>
   <si>
+    <t>Jr</t>
+  </si>
+  <si>
     <t>May 1, 1995</t>
   </si>
   <si>
@@ -268,7 +355,7 @@
     <t>Contact Number</t>
   </si>
   <si>
-    <t>Profile_0030</t>
+    <t>Profile_0031</t>
   </si>
   <si>
     <t>00123 Ortigas Pasig City</t>
@@ -295,13 +382,7 @@
     <t>Degree</t>
   </si>
   <si>
-    <t>From Year</t>
-  </si>
-  <si>
-    <t>To Year</t>
-  </si>
-  <si>
-    <t>Profile_0031</t>
+    <t>Profile_0032</t>
   </si>
   <si>
     <t>STI College Ortigas-Cainta</t>
@@ -310,13 +391,7 @@
     <t>Bachelor of Science in Information Technology</t>
   </si>
   <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>Profile_0032</t>
+    <t>Profile_0033</t>
   </si>
   <si>
     <t>FEU Manila</t>
@@ -325,7 +400,115 @@
     <t>Masteral in Information Technology</t>
   </si>
   <si>
-    <t>2019</t>
+    <t>Profile_0034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company </t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Work Accomplishments</t>
+  </si>
+  <si>
+    <t>Certificates Received</t>
+  </si>
+  <si>
+    <t>Professional Skills</t>
+  </si>
+  <si>
+    <t>Profile_0035</t>
+  </si>
+  <si>
+    <t>WOG</t>
+  </si>
+  <si>
+    <t>Research Department</t>
+  </si>
+  <si>
+    <t>QA Tester/Project Secretary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA </t>
+  </si>
+  <si>
+    <t>Manual Testing Training</t>
+  </si>
+  <si>
+    <t>Profile_0036</t>
+  </si>
+  <si>
+    <t>Web Outsourcing Gateway</t>
+  </si>
+  <si>
+    <t>QA Department</t>
+  </si>
+  <si>
+    <t>Testing web and mobile application</t>
+  </si>
+  <si>
+    <t>Manual and Automation Testing Training</t>
+  </si>
+  <si>
+    <t>Software tester, Automation skills</t>
+  </si>
+  <si>
+    <t>Profile_0037</t>
+  </si>
+  <si>
+    <t>Profile_0038</t>
+  </si>
+  <si>
+    <t>Profile_0039</t>
+  </si>
+  <si>
+    <t>Profile_0040</t>
+  </si>
+  <si>
+    <t>Profile_0041</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Profile_0042</t>
+  </si>
+  <si>
+    <t>Portable Document File Sample.pdf</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Profile_0043</t>
+  </si>
+  <si>
+    <t>Sample File</t>
+  </si>
+  <si>
+    <t>Profile_0044</t>
+  </si>
+  <si>
+    <t>Colleague Name or Group Name</t>
+  </si>
+  <si>
+    <t>Profile_0045</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Profile_0046</t>
+  </si>
+  <si>
+    <t>This file has been shared via email.</t>
+  </si>
+  <si>
+    <t>Profile_0047</t>
   </si>
 </sst>
 </file>
@@ -334,9 +517,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -363,6 +546,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -377,21 +574,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,8 +587,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -426,9 +617,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -437,6 +627,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,14 +655,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -481,22 +670,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,6 +681,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,7 +710,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,7 +740,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,25 +776,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,43 +860,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,79 +884,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,6 +901,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -754,17 +957,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -795,15 +987,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -821,7 +1004,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -839,135 +1022,139 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -980,17 +1167,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1001,38 +1184,30 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,7 +1530,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1366,13 +1541,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1380,7 +1555,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -1391,13 +1566,13 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1413,7 +1588,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
@@ -1424,7 +1599,7 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
@@ -1446,98 +1621,718 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.8571428571429" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5714285714286" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7142857142857" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44.4285714285714" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.8571428571429" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.2857142857143" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.14285714285714" style="1"/>
+    <col min="1" max="1" width="24" style="9" customWidth="1"/>
+    <col min="2" max="2" width="33.8571428571429" style="9" customWidth="1"/>
+    <col min="3" max="4" width="31.5714285714286" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26.8571428571429" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.8571428571429" style="9" customWidth="1"/>
+    <col min="7" max="7" width="30.1428571428571" style="9" customWidth="1"/>
+    <col min="8" max="8" width="26.5714285714286" style="9" customWidth="1"/>
+    <col min="9" max="9" width="33" style="9" customWidth="1"/>
+    <col min="10" max="10" width="32.7142857142857" style="9" customWidth="1"/>
+    <col min="11" max="16384" width="9.14285714285714" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
-        <v>92</v>
+      <c r="D1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>100</v>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="21" style="5" customWidth="1"/>
+    <col min="2" max="2" width="26.8571428571429" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25.5714285714286" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.7142857142857" style="5" customWidth="1"/>
+    <col min="5" max="5" width="44.4285714285714" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.14285714285714" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
     <hyperlink ref="B3" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="23.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="26.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="25.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="25.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="27.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="34.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="33.5714285714286" customWidth="1"/>
+    <col min="8" max="8" width="37.7142857142857" customWidth="1"/>
+    <col min="9" max="9" width="38.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="16.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="23.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="20.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="21.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="25.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="40.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="19.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="14.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="33.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="31.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="24.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com" tooltip="mailto:marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="16.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="23.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="22.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com" tooltip="mailto:marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="20.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="25.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="41.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="25.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="27.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="26.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="40.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="35.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="20.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="28.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1547,10 +2342,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1564,165 +2359,245 @@
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:7">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="B2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="6"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="6"/>
+      <c r="B3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="B4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="B5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="B6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" customFormat="1" spans="1:7">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="23" t="s">
+      <c r="B7" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="B8" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9" t="s">
         <v>34</v>
       </c>
+    </row>
+    <row r="10" ht="45" spans="1:4">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" ht="90" spans="1:5">
+      <c r="A15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1734,6 +2609,12 @@
     <hyperlink ref="B6" r:id="rId1" display="marymary@gmail.com"/>
     <hyperlink ref="B8" r:id="rId1" display="marymary@gmail.com"/>
     <hyperlink ref="B9" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B11" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B12" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B13" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B14" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B15" r:id="rId1" display="marymary@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1743,102 +2624,162 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:H3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="22.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="24.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="22.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="29.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="38.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="26.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="20.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="16.5714285714286" customWidth="1"/>
-    <col min="8" max="8" width="16.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="21.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="19.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1" spans="1:8">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="F1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="2" ht="45" spans="1:8">
+      <c r="A2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" ht="30" spans="1:8">
+      <c r="A3" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" ht="30" spans="1:8">
+      <c r="A5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
     <hyperlink ref="B3" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId1" display="marymary@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1851,60 +2792,75 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="26.4285714285714" style="15" customWidth="1"/>
-    <col min="2" max="2" width="24.7142857142857" style="15" customWidth="1"/>
-    <col min="3" max="3" width="25.4285714285714" style="15" customWidth="1"/>
-    <col min="4" max="4" width="24.5714285714286" style="15" customWidth="1"/>
-    <col min="5" max="5" width="11.2857142857143" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="9.14285714285714" style="15"/>
+    <col min="1" max="1" width="26.4285714285714" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.7142857142857" style="17" customWidth="1"/>
+    <col min="3" max="3" width="25.4285714285714" style="17" customWidth="1"/>
+    <col min="4" max="4" width="24.5714285714286" style="17" customWidth="1"/>
+    <col min="5" max="5" width="11.2857142857143" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="9.14285714285714" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>49</v>
+      <c r="D1" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>52</v>
+      <c r="A2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="18"/>
+      <c r="D4" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="marymary@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1944,37 +2900,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>54</v>
+      <c r="D1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>58</v>
+      <c r="A2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1989,13 +2945,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="26.5714285714286" customWidth="1"/>
@@ -2004,20 +2960,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>59</v>
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2026,10 +3014,57 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="20.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="27.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="28.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2047,157 +3082,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>66</v>
+      <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>71</v>
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="marymary@gmail.com"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
-  <cols>
-    <col min="1" max="1" width="24" style="6" customWidth="1"/>
-    <col min="2" max="2" width="33.8571428571429" style="6" customWidth="1"/>
-    <col min="3" max="4" width="31.5714285714286" style="6" customWidth="1"/>
-    <col min="5" max="5" width="26.8571428571429" style="6" customWidth="1"/>
-    <col min="6" max="6" width="20.8571428571429" style="6" customWidth="1"/>
-    <col min="7" max="7" width="30.1428571428571" style="6" customWidth="1"/>
-    <col min="8" max="8" width="26.5714285714286" style="6" customWidth="1"/>
-    <col min="9" max="9" width="33" style="6" customWidth="1"/>
-    <col min="10" max="10" width="32.7142857142857" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9.14285714285714" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>